<commit_message>
Encapsulated couple functions (algorithms); Fixed get_lagged buggy lines; fixed maep to show percentage; added csv results; more
</commit_message>
<xml_diff>
--- a/results/results_emd_40cv_1day.xlsx
+++ b/results/results_emd_40cv_1day.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marko\code\ML-Load-Forecasting\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDFA92A8-BD83-48E1-A149-CCC8B48B544F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF9950B8-113B-4DCB-A25A-DEDB2B8D07FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{073BCCA1-CE2F-4E6B-85C8-A01B76F2D396}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="ISO-NE" sheetId="3" r:id="rId3"/>
+    <sheet name="ONS" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="246">
   <si>
     <t>IMF_0</t>
   </si>
@@ -526,6 +526,246 @@
   </si>
   <si>
     <t>5.51 (+- 2.66)</t>
+  </si>
+  <si>
+    <t>0.8153 (+- 0.1850)</t>
+  </si>
+  <si>
+    <t>0.8073 (+- 0.1931)</t>
+  </si>
+  <si>
+    <t>1889.4 (+- 909.88)</t>
+  </si>
+  <si>
+    <t>1540.3 (+- 758.01)</t>
+  </si>
+  <si>
+    <t>0.8282 (+- 0.1746)</t>
+  </si>
+  <si>
+    <t>0.8207 (+- 0.1823)</t>
+  </si>
+  <si>
+    <t>1808.7 (+- 899.29)</t>
+  </si>
+  <si>
+    <t>1468.9 (+- 727.58)</t>
+  </si>
+  <si>
+    <t>4.18 (+- 2.13)</t>
+  </si>
+  <si>
+    <t>4.13 (+- 2.05)</t>
+  </si>
+  <si>
+    <t>4.38 (+- 2.23)</t>
+  </si>
+  <si>
+    <t>4.33 (+- 2.14)</t>
+  </si>
+  <si>
+    <t>0.7755 (+- 0.1906)</t>
+  </si>
+  <si>
+    <t>0.7656 (+- 0.1989)</t>
+  </si>
+  <si>
+    <t>2145.9 (+- 898.08)</t>
+  </si>
+  <si>
+    <t>1735.7 (+- 744.81)</t>
+  </si>
+  <si>
+    <t>4.99 (+- 2.24)</t>
+  </si>
+  <si>
+    <t>4.92 (+- 2.11)</t>
+  </si>
+  <si>
+    <t>0.8450 (+- 0.1748)</t>
+  </si>
+  <si>
+    <t>0.8382 (+- 0.1824)</t>
+  </si>
+  <si>
+    <t>1678.2 (+- 935.67)</t>
+  </si>
+  <si>
+    <t>1365.5 (+- 789.88)</t>
+  </si>
+  <si>
+    <t>3.88 (+- 2.25)</t>
+  </si>
+  <si>
+    <t>3.83 (+- 2.19)</t>
+  </si>
+  <si>
+    <t>0.8365 (+- 0.1756)</t>
+  </si>
+  <si>
+    <t>0.8294 (+- 0.1833)</t>
+  </si>
+  <si>
+    <t>1759.6 (+- 886.85)</t>
+  </si>
+  <si>
+    <t>1434.0 (+- 739.77)</t>
+  </si>
+  <si>
+    <t>4.07 (+- 2.16)</t>
+  </si>
+  <si>
+    <t>4.03 (+- 2.08)</t>
+  </si>
+  <si>
+    <t>Decomposition</t>
+  </si>
+  <si>
+    <t>0.8377 (+- 0.1106)</t>
+  </si>
+  <si>
+    <t>0.3999 (+- 0.7667)</t>
+  </si>
+  <si>
+    <t>0.3697 (+- 0.8052)</t>
+  </si>
+  <si>
+    <t>0.1390 (+- 0.0705)</t>
+  </si>
+  <si>
+    <t>0.1093 (+- 0.0559)</t>
+  </si>
+  <si>
+    <t>503.72 (+- 894.44)</t>
+  </si>
+  <si>
+    <t>77.31 (+- 33.05)</t>
+  </si>
+  <si>
+    <t>0.9309 (+- 0.0464)</t>
+  </si>
+  <si>
+    <t>0.6013 (+- 0.4957)</t>
+  </si>
+  <si>
+    <t>0.5812 (+- 0.5206)</t>
+  </si>
+  <si>
+    <t>0.3067 (+- 0.1758)</t>
+  </si>
+  <si>
+    <t>0.2408 (+- 0.1418)</t>
+  </si>
+  <si>
+    <t>314.04 (+- 820.27)</t>
+  </si>
+  <si>
+    <t>65.84 (+- 28.01)</t>
+  </si>
+  <si>
+    <t>0.8339 (+- 0.0774)</t>
+  </si>
+  <si>
+    <t>-5.0926 (+- 16.2232)</t>
+  </si>
+  <si>
+    <t>-5.3991 (+- 17.0395)</t>
+  </si>
+  <si>
+    <t>0.2844 (+- 0.1653)</t>
+  </si>
+  <si>
+    <t>0.2254 (+- 0.1331)</t>
+  </si>
+  <si>
+    <t>615.55 (+- 862.49)</t>
+  </si>
+  <si>
+    <t>139.59 (+- 28.39)</t>
+  </si>
+  <si>
+    <t>0.7995 (+- 0.0751)</t>
+  </si>
+  <si>
+    <t>-0.6542 (+- 0.9259)</t>
+  </si>
+  <si>
+    <t>-0.7374 (+- 0.9725)</t>
+  </si>
+  <si>
+    <t>0.1786 (+- 0.0935)</t>
+  </si>
+  <si>
+    <t>0.1479 (+- 0.0774)</t>
+  </si>
+  <si>
+    <t>369.15 (+- 375.11)</t>
+  </si>
+  <si>
+    <t>142.40 (+- 19.79)</t>
+  </si>
+  <si>
+    <t>0.9308 (+- 0.0359)</t>
+  </si>
+  <si>
+    <t>-1.0895 (+- 2.6996)</t>
+  </si>
+  <si>
+    <t>-1.1946 (+- 2.8354)</t>
+  </si>
+  <si>
+    <t>0.2144 (+- 0.0863)</t>
+  </si>
+  <si>
+    <t>0.1816 (+- 0.0764)</t>
+  </si>
+  <si>
+    <t>664.20 (+- 1834.49)</t>
+  </si>
+  <si>
+    <t>133.67 (+- 25.11)</t>
+  </si>
+  <si>
+    <t>0.9788 (+- 0.0093)</t>
+  </si>
+  <si>
+    <t>-0.9066 (+- 2.1016)</t>
+  </si>
+  <si>
+    <t>-1.0025 (+- 2.2073)</t>
+  </si>
+  <si>
+    <t>0.2197 (+- 0.1334)</t>
+  </si>
+  <si>
+    <t>0.1910 (+- 0.1184)</t>
+  </si>
+  <si>
+    <t>367.39 (+- 382.03)</t>
+  </si>
+  <si>
+    <t>128.35 (+- 33.99)</t>
+  </si>
+  <si>
+    <t>0.9961 (+- 0.0038)</t>
+  </si>
+  <si>
+    <t>-33.3577 (+- 73.4038)</t>
+  </si>
+  <si>
+    <t>-35.0864 (+- 77.0970)</t>
+  </si>
+  <si>
+    <t>0.2904 (+- 0.1744)</t>
+  </si>
+  <si>
+    <t>0.2523 (+- 0.1569)</t>
+  </si>
+  <si>
+    <t>340.19 (+- 741.16)</t>
+  </si>
+  <si>
+    <t>80.36 (+- 51.14)</t>
   </si>
 </sst>
 </file>
@@ -572,12 +812,10 @@
       <family val="3"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <color rgb="FFCDA48C"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -649,9 +887,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -661,9 +896,14 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -983,7 +1223,7 @@
   <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1444,7 +1684,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:G26"/>
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1873,15 +2113,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0382A149-1E28-46FD-B8C5-6B5FA287F02E}">
-  <dimension ref="B3:I34"/>
+  <dimension ref="B3:J44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:I8"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="9" width="18.7109375" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
@@ -2072,7 +2313,7 @@
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
         <v>155</v>
       </c>
@@ -2098,7 +2339,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="13" t="s">
         <v>156</v>
       </c>
@@ -2124,7 +2365,7 @@
         <v>2.46E-2</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="13" t="s">
         <v>124</v>
       </c>
@@ -2150,33 +2391,33 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="13" t="s">
         <v>130</v>
       </c>
       <c r="C20" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="D20" s="21">
+      <c r="D20" s="20">
         <v>0.94569999999999999</v>
       </c>
-      <c r="E20" s="21">
+      <c r="E20" s="20">
         <v>0.91859999999999997</v>
       </c>
-      <c r="F20" s="22">
+      <c r="F20" s="21">
         <v>450.261098</v>
       </c>
-      <c r="G20" s="22">
+      <c r="G20" s="21">
         <v>399.17117200000001</v>
       </c>
-      <c r="H20" s="20">
+      <c r="H20" s="19">
         <v>3.1399999999999997E-2</v>
       </c>
-      <c r="I20" s="20">
+      <c r="I20" s="19">
         <v>3.0800000000000001E-2</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="13" t="s">
         <v>66</v>
       </c>
@@ -2202,7 +2443,7 @@
         <v>3.7499999999999999E-2</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="13" t="s">
         <v>157</v>
       </c>
@@ -2215,10 +2456,10 @@
       <c r="E22" s="13">
         <v>0.9456</v>
       </c>
-      <c r="F22" s="24">
+      <c r="F22" s="22">
         <v>368.06040999999999</v>
       </c>
-      <c r="G22" s="24">
+      <c r="G22" s="22">
         <v>290.00559900000002</v>
       </c>
       <c r="H22" s="16">
@@ -2228,47 +2469,276 @@
         <v>2.1899999999999999E-2</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="G24" s="18"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="23"/>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="23"/>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F28" s="18"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="23"/>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F29" s="18"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="23"/>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F30" s="18"/>
-      <c r="G30" s="3"/>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F31" s="18"/>
-      <c r="G31" s="7"/>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="G32" s="7"/>
-    </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G33" s="3"/>
-    </row>
-    <row r="34" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G34" s="3"/>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H26" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="I26" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="J26" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="D27" s="23" t="s">
+        <v>197</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="G27" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="H27" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="I27" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="J27" s="23" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B28" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="D28" s="23" t="s">
+        <v>204</v>
+      </c>
+      <c r="E28" s="23" t="s">
+        <v>205</v>
+      </c>
+      <c r="F28" s="23" t="s">
+        <v>206</v>
+      </c>
+      <c r="G28" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="H28" s="23" t="s">
+        <v>208</v>
+      </c>
+      <c r="I28" s="23" t="s">
+        <v>209</v>
+      </c>
+      <c r="J28" s="23" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B29" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="D29" s="23" t="s">
+        <v>211</v>
+      </c>
+      <c r="E29" s="23" t="s">
+        <v>212</v>
+      </c>
+      <c r="F29" s="23" t="s">
+        <v>213</v>
+      </c>
+      <c r="G29" s="23" t="s">
+        <v>214</v>
+      </c>
+      <c r="H29" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="I29" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="J29" s="23" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="D30" s="23" t="s">
+        <v>218</v>
+      </c>
+      <c r="E30" s="23" t="s">
+        <v>219</v>
+      </c>
+      <c r="F30" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="G30" s="23" t="s">
+        <v>221</v>
+      </c>
+      <c r="H30" s="23" t="s">
+        <v>222</v>
+      </c>
+      <c r="I30" s="23" t="s">
+        <v>223</v>
+      </c>
+      <c r="J30" s="23" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>225</v>
+      </c>
+      <c r="E31" s="23" t="s">
+        <v>226</v>
+      </c>
+      <c r="F31" s="23" t="s">
+        <v>227</v>
+      </c>
+      <c r="G31" s="23" t="s">
+        <v>228</v>
+      </c>
+      <c r="H31" s="23" t="s">
+        <v>229</v>
+      </c>
+      <c r="I31" s="23" t="s">
+        <v>230</v>
+      </c>
+      <c r="J31" s="23" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B32" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="D32" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="E32" s="23" t="s">
+        <v>233</v>
+      </c>
+      <c r="F32" s="23" t="s">
+        <v>234</v>
+      </c>
+      <c r="G32" s="23" t="s">
+        <v>235</v>
+      </c>
+      <c r="H32" s="23" t="s">
+        <v>236</v>
+      </c>
+      <c r="I32" s="23" t="s">
+        <v>237</v>
+      </c>
+      <c r="J32" s="23" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B33" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="D33" s="23" t="s">
+        <v>239</v>
+      </c>
+      <c r="E33" s="23" t="s">
+        <v>240</v>
+      </c>
+      <c r="F33" s="23" t="s">
+        <v>241</v>
+      </c>
+      <c r="G33" s="23" t="s">
+        <v>242</v>
+      </c>
+      <c r="H33" s="23" t="s">
+        <v>243</v>
+      </c>
+      <c r="I33" s="23" t="s">
+        <v>244</v>
+      </c>
+      <c r="J33" s="23" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D34" s="24"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D35" s="24"/>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D36" s="24"/>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D37" s="24"/>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D38" s="24"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D39" s="24"/>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D40" s="24"/>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D41" s="24"/>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D42" s="24"/>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D43" s="24"/>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D44" s="24"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -2276,14 +2746,364 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65330A7C-F172-4A02-96B9-81FC7BF2ACB5}">
-  <dimension ref="A1"/>
+  <dimension ref="B3:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:I20"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="8" width="18" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>193</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="I4" s="23" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="I5" s="23" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="G6" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="H6" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="I6" s="23" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="I7" s="23" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="H8" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="I8" s="23" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="D18" s="13">
+        <v>0.98270000000000002</v>
+      </c>
+      <c r="E18" s="13">
+        <v>0.97689999999999999</v>
+      </c>
+      <c r="F18" s="22">
+        <v>587.77479400000004</v>
+      </c>
+      <c r="G18" s="22">
+        <v>505.100956</v>
+      </c>
+      <c r="H18" s="16">
+        <v>1.32E-2</v>
+      </c>
+      <c r="I18" s="16">
+        <v>1.3299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="D19" s="13">
+        <v>0.97809999999999997</v>
+      </c>
+      <c r="E19" s="13">
+        <v>0.9708</v>
+      </c>
+      <c r="F19" s="22">
+        <v>660.44841399999996</v>
+      </c>
+      <c r="G19" s="22">
+        <v>587.03580499999998</v>
+      </c>
+      <c r="H19" s="16">
+        <v>1.6199999999999999E-2</v>
+      </c>
+      <c r="I19" s="16">
+        <v>1.6299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="D20" s="20">
+        <v>0.80179999999999996</v>
+      </c>
+      <c r="E20" s="20">
+        <v>0.73570000000000002</v>
+      </c>
+      <c r="F20" s="21">
+        <v>1988.0123000000001</v>
+      </c>
+      <c r="G20" s="21">
+        <v>1886.3241459999999</v>
+      </c>
+      <c r="H20" s="19">
+        <v>5.16E-2</v>
+      </c>
+      <c r="I20" s="19">
+        <v>5.0099999999999999E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="D21" s="13">
+        <v>0.88080000000000003</v>
+      </c>
+      <c r="E21" s="13">
+        <v>0.84099999999999997</v>
+      </c>
+      <c r="F21" s="22">
+        <v>1541.7415100000001</v>
+      </c>
+      <c r="G21" s="22">
+        <v>1334.4457010000001</v>
+      </c>
+      <c r="H21" s="16">
+        <v>3.8300000000000001E-2</v>
+      </c>
+      <c r="I21" s="16">
+        <v>3.73E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="D22" s="13">
+        <v>0.97529999999999994</v>
+      </c>
+      <c r="E22" s="13">
+        <v>0.96709999999999996</v>
+      </c>
+      <c r="F22" s="22">
+        <v>701.29605500000002</v>
+      </c>
+      <c r="G22" s="22">
+        <v>568.38252</v>
+      </c>
+      <c r="H22" s="16">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I22" s="16">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>